<commit_message>
add icons for errors
</commit_message>
<xml_diff>
--- a/app/static/results.xlsx
+++ b/app/static/results.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,19 +51,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -364,14 +364,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+    <col customWidth="1" max="5" min="5" width="15"/>
+    <col customWidth="1" max="6" min="6" width="15"/>
+    <col customWidth="1" max="7" min="7" width="15"/>
+    <col customWidth="1" max="8" min="8" width="15"/>
+    <col customWidth="1" max="9" min="9" width="15"/>
+    <col customWidth="1" max="10" min="10" width="15"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="E6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -570,13 +570,13 @@
         </is>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="E10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
@@ -615,10 +615,10 @@
         <v>4</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more template events
</commit_message>
<xml_diff>
--- a/app/static/results.xlsx
+++ b/app/static/results.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:J10"/>
+  <dimension ref="C3:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -612,10 +612,190 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>Политика №10</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>Задание №10</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Политика №11</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>Задание №11</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>Политика №12</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Задание №12</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="1" t="n">
-        <v>4</v>
+      <c r="H13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>Политика №13</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>Задание №13</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>Политика №14</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>Задание №14</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Политика №15</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>Задание №15</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add alternative task check, create table for protected documents
</commit_message>
<xml_diff>
--- a/app/static/results.xlsx
+++ b/app/static/results.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,19 +51,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:J16"/>
+  <dimension ref="C3:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,14 +364,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-    <col customWidth="1" max="5" min="5" width="15"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
-    <col customWidth="1" max="8" min="8" width="15"/>
-    <col customWidth="1" max="9" min="9" width="15"/>
-    <col customWidth="1" max="10" min="10" width="15"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0</v>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -453,19 +453,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -483,19 +483,19 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -549,13 +549,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -750,22 +750,22 @@
         </is>
       </c>
       <c r="E15" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -798,7 +798,278 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>Ложные объекты</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>Отсутствующие объекты</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>Итого недочетов</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №4</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Задание №4</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №5</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>Задание №5</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №6</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>Задание №6</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №7</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>Задание №7</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №8</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Задание №8</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №9</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Задание №9</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №10</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Задание №10</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №11</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Задание №11</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №12</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Задание №12</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №13</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Задание №13</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №14</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>Задание №14</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>Объект защиты №15</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>Задание №15</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
display wrong verdict and violation level in results
</commit_message>
<xml_diff>
--- a/app/static/results.xlsx
+++ b/app/static/results.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:J31"/>
+  <dimension ref="C3:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -372,6 +372,8 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -379,30 +381,40 @@
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="2" t="inlineStr">
         <is>
+          <t>Ложные политики</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Отсутствующие политики</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Ложные объекты</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Отсутствующие объекты</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
           <t>Ложные теги</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Ложные политики</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>Отсутствующие политики</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Ложные объекты</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>Отсутствующие объекты</t>
-        </is>
-      </c>
       <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>Ложные вердикты</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Ложные уровни нарушения</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>Итого недочетов</t>
         </is>
@@ -420,10 +432,10 @@
         </is>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0</v>
@@ -432,9 +444,15 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
         <v>6</v>
       </c>
     </row>
@@ -450,22 +468,28 @@
         </is>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="H5" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -480,7 +504,7 @@
         </is>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0</v>
@@ -492,9 +516,15 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -519,12 +549,18 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -540,22 +576,28 @@
         </is>
       </c>
       <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="J8" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -587,6 +629,12 @@
       <c r="J9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="K9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="C10" s="1" t="inlineStr">
@@ -617,6 +665,12 @@
       <c r="J10" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="K10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="C11" s="1" t="inlineStr">
@@ -647,6 +701,12 @@
       <c r="J11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="K11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="C12" s="1" t="inlineStr">
@@ -677,6 +737,12 @@
       <c r="J12" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="K12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="C13" s="1" t="inlineStr">
@@ -690,22 +756,28 @@
         </is>
       </c>
       <c r="E13" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -720,22 +792,28 @@
         </is>
       </c>
       <c r="E14" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -750,21 +828,27 @@
         </is>
       </c>
       <c r="E15" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="n">
         <v>6</v>
       </c>
     </row>
@@ -795,7 +879,13 @@
         <v>0</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -895,10 +985,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1042,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">

</xml_diff>